<commit_message>
some changes + new data for TMAP NTC
</commit_message>
<xml_diff>
--- a/olíuþrýstingur_viðnámsmælingar.xlsx
+++ b/olíuþrýstingur_viðnámsmælingar.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>bar</t>
   </si>
@@ -33,6 +33,18 @@
   </si>
   <si>
     <t>Ωavg</t>
+  </si>
+  <si>
+    <t>vref</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>Ω</t>
   </si>
 </sst>
 </file>
@@ -874,6 +886,416 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="is-IS"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.8851487314085739E-2"/>
+                  <c:y val="-4.4349664625255173E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="is-IS"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$7:$H$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$7:$L$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>4.995004995004995E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2688863602631968E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9224485778958756E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12099921935987511</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16207063376874697</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.212562236690923</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.24760003801919972</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.28768672541350548</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3362559462736685</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.36951287275421374</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.40757749712973596</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.44502140839938048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.48634619724667116</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.52212072362529105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="424244192"/>
+        <c:axId val="424245368"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="424244192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="is-IS"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="424245368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="424245368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="is-IS"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="424244192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="is-IS"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -954,6 +1376,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1986,20 +2448,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>3810</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>407670</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>29527</xdr:rowOff>
+      <xdr:rowOff>37147</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>308610</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>102870</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>98107</xdr:rowOff>
+      <xdr:rowOff>105727</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2020,16 +2998,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>115252</xdr:rowOff>
+      <xdr:rowOff>145732</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>952</xdr:rowOff>
+      <xdr:rowOff>31432</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2043,6 +3021,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2314,15 +3322,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="H6:K20"/>
+  <dimension ref="H2:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L7" activeCellId="1" sqref="H7:H20 L7:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="6" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3">
+        <v>1000</v>
+      </c>
+      <c r="L3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H6" t="s">
         <v>0</v>
       </c>
@@ -2336,7 +3366,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H7">
         <v>0</v>
       </c>
@@ -2350,8 +3380,12 @@
         <f>(I7+J7)/2</f>
         <v>1</v>
       </c>
+      <c r="L7">
+        <f>$K$2*K7/($K$3+K7)</f>
+        <v>4.995004995004995E-3</v>
+      </c>
     </row>
-    <row r="8" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H8">
         <v>0.5</v>
       </c>
@@ -2365,8 +3399,12 @@
         <f>(I8+J8)/2</f>
         <v>10.65</v>
       </c>
+      <c r="L8">
+        <f t="shared" ref="L8:L20" si="0">$K$2*K8/($K$3+K8)</f>
+        <v>5.2688863602631968E-2</v>
+      </c>
     </row>
-    <row r="9" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H9">
         <v>1</v>
       </c>
@@ -2377,11 +3415,15 @@
         <v>16.100000000000001</v>
       </c>
       <c r="K9">
-        <f t="shared" ref="K8:K20" si="0">(I9+J9)/2</f>
+        <f t="shared" ref="K8:K20" si="1">(I9+J9)/2</f>
         <v>16.100000000000001</v>
       </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>7.9224485778958756E-2</v>
+      </c>
     </row>
-    <row r="10" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H10">
         <v>1.5</v>
       </c>
@@ -2392,11 +3434,15 @@
         <v>24.8</v>
       </c>
       <c r="K10">
+        <f t="shared" si="1"/>
+        <v>24.8</v>
+      </c>
+      <c r="L10">
         <f t="shared" si="0"/>
-        <v>24.8</v>
+        <v>0.12099921935987511</v>
       </c>
     </row>
-    <row r="11" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H11">
         <v>2</v>
       </c>
@@ -2407,11 +3453,15 @@
         <v>33.5</v>
       </c>
       <c r="K11">
+        <f t="shared" si="1"/>
+        <v>33.5</v>
+      </c>
+      <c r="L11">
         <f t="shared" si="0"/>
-        <v>33.5</v>
+        <v>0.16207063376874697</v>
       </c>
     </row>
-    <row r="12" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H12">
         <v>2.5</v>
       </c>
@@ -2422,11 +3472,15 @@
         <v>44.4</v>
       </c>
       <c r="K12">
+        <f t="shared" si="1"/>
+        <v>44.4</v>
+      </c>
+      <c r="L12">
         <f t="shared" si="0"/>
-        <v>44.4</v>
+        <v>0.212562236690923</v>
       </c>
     </row>
-    <row r="13" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H13">
         <v>3</v>
       </c>
@@ -2437,11 +3491,15 @@
         <v>53.2</v>
       </c>
       <c r="K13">
+        <f t="shared" si="1"/>
+        <v>52.1</v>
+      </c>
+      <c r="L13">
         <f t="shared" si="0"/>
-        <v>52.1</v>
+        <v>0.24760003801919972</v>
       </c>
     </row>
-    <row r="14" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H14">
         <v>3.5</v>
       </c>
@@ -2452,11 +3510,15 @@
         <v>62.1</v>
       </c>
       <c r="K14">
+        <f t="shared" si="1"/>
+        <v>61.05</v>
+      </c>
+      <c r="L14">
         <f t="shared" si="0"/>
-        <v>61.05</v>
+        <v>0.28768672541350548</v>
       </c>
     </row>
-    <row r="15" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H15">
         <v>4</v>
       </c>
@@ -2467,11 +3529,15 @@
         <v>71</v>
       </c>
       <c r="K15">
+        <f t="shared" si="1"/>
+        <v>72.099999999999994</v>
+      </c>
+      <c r="L15">
         <f t="shared" si="0"/>
-        <v>72.099999999999994</v>
+        <v>0.3362559462736685</v>
       </c>
     </row>
-    <row r="16" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H16">
         <v>4.5</v>
       </c>
@@ -2482,11 +3548,15 @@
         <v>79.8</v>
       </c>
       <c r="K16">
+        <f t="shared" si="1"/>
+        <v>79.8</v>
+      </c>
+      <c r="L16">
         <f t="shared" si="0"/>
-        <v>79.8</v>
+        <v>0.36951287275421374</v>
       </c>
     </row>
-    <row r="17" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H17">
         <v>5</v>
       </c>
@@ -2497,11 +3567,15 @@
         <v>88.7</v>
       </c>
       <c r="K17">
+        <f t="shared" si="1"/>
+        <v>88.75</v>
+      </c>
+      <c r="L17">
         <f t="shared" si="0"/>
-        <v>88.75</v>
+        <v>0.40757749712973596</v>
       </c>
     </row>
-    <row r="18" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H18">
         <v>5.5</v>
       </c>
@@ -2512,11 +3586,15 @@
         <v>97.7</v>
       </c>
       <c r="K18">
+        <f t="shared" si="1"/>
+        <v>97.7</v>
+      </c>
+      <c r="L18">
         <f t="shared" si="0"/>
-        <v>97.7</v>
+        <v>0.44502140839938048</v>
       </c>
     </row>
-    <row r="19" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H19">
         <v>6</v>
       </c>
@@ -2527,11 +3605,15 @@
         <v>106.6</v>
       </c>
       <c r="K19">
+        <f t="shared" si="1"/>
+        <v>107.75</v>
+      </c>
+      <c r="L19">
         <f t="shared" si="0"/>
-        <v>107.75</v>
+        <v>0.48634619724667116</v>
       </c>
     </row>
-    <row r="20" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H20">
         <v>6.5</v>
       </c>
@@ -2542,8 +3624,20 @@
         <v>115.5</v>
       </c>
       <c r="K20">
+        <f t="shared" si="1"/>
+        <v>116.6</v>
+      </c>
+      <c r="L20">
         <f t="shared" si="0"/>
-        <v>116.6</v>
+        <v>0.52212072362529105</v>
+      </c>
+    </row>
+    <row r="22" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H22">
+        <v>10</v>
+      </c>
+      <c r="K22">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rpm mælingar m. interrupt og fleira data
</commit_message>
<xml_diff>
--- a/olíuþrýstingur_viðnámsmælingar.xlsx
+++ b/olíuþrýstingur_viðnámsmælingar.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1644" yWindow="0" windowWidth="15408" windowHeight="9300"/>
+    <workbookView xWindow="3288" yWindow="0" windowWidth="15408" windowHeight="9300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -298,11 +298,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="424247328"/>
-        <c:axId val="424248112"/>
+        <c:axId val="425460224"/>
+        <c:axId val="425455520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="424247328"/>
+        <c:axId val="425460224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -359,12 +359,12 @@
             <a:endParaRPr lang="is-IS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424248112"/>
+        <c:crossAx val="425455520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="424248112"/>
+        <c:axId val="425455520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -421,7 +421,7 @@
             <a:endParaRPr lang="is-IS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424247328"/>
+        <c:crossAx val="425460224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -714,11 +714,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="424257128"/>
-        <c:axId val="424257912"/>
+        <c:axId val="425458656"/>
+        <c:axId val="424256736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="424257128"/>
+        <c:axId val="425458656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -775,12 +775,12 @@
             <a:endParaRPr lang="is-IS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424257912"/>
+        <c:crossAx val="424256736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="424257912"/>
+        <c:axId val="424256736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -837,7 +837,7 @@
             <a:endParaRPr lang="is-IS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424257128"/>
+        <c:crossAx val="425458656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1124,11 +1124,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="424244192"/>
-        <c:axId val="424245368"/>
+        <c:axId val="424257128"/>
+        <c:axId val="424258304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="424244192"/>
+        <c:axId val="424257128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1185,12 +1185,12 @@
             <a:endParaRPr lang="is-IS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424245368"/>
+        <c:crossAx val="424258304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="424245368"/>
+        <c:axId val="424258304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1247,7 +1247,7 @@
             <a:endParaRPr lang="is-IS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424244192"/>
+        <c:crossAx val="424257128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3028,16 +3028,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3324,8 +3324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="H2:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L7" activeCellId="1" sqref="H7:H20 L7:L20"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3415,7 +3415,7 @@
         <v>16.100000000000001</v>
       </c>
       <c r="K9">
-        <f t="shared" ref="K8:K20" si="1">(I9+J9)/2</f>
+        <f t="shared" ref="K9:K20" si="1">(I9+J9)/2</f>
         <v>16.100000000000001</v>
       </c>
       <c r="L9">

</xml_diff>